<commit_message>
23 dec 2023 update
</commit_message>
<xml_diff>
--- a/Financials.xlsx
+++ b/Financials.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="20640" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Investments" sheetId="13" r:id="rId1"/>
     <sheet name="BalanceSheet" sheetId="12" r:id="rId2"/>
     <sheet name="Expenses" sheetId="14" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Balance Sheet</t>
   </si>
@@ -238,16 +238,22 @@
   <si>
     <t>Stationary</t>
   </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>Saturday,December 23,2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,9 +423,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,7 +433,7 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -436,16 +442,16 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -473,16 +479,16 @@
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -491,7 +497,22 @@
     <xf numFmtId="1" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,18 +531,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -807,31 +816,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="37" style="4" customWidth="1"/>
     <col min="5" max="5" width="29" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="16.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1">
+    <row r="2" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
@@ -841,69 +851,69 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="22.5" customHeight="1">
+    <row r="4" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="22.5" customHeight="1">
+    <row r="5" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="6">
-        <f>SUM(E13:E19)</f>
-        <v>117500</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="22.5" customHeight="1">
+        <f>SUM(E13:E21)</f>
+        <v>142500</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="19">
-        <f>SUM(E21:E25)</f>
+        <f>SUM(E23:E27)</f>
         <v>17380</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="22.5" customHeight="1">
+    <row r="7" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="2:5" ht="22.5" customHeight="1">
+    <row r="9" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="22">
-        <f>SUM(E12:E25)</f>
-        <v>134880</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15">
+        <f>SUM(E12:E27)</f>
+        <v>159880</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="2:5" ht="22.5" customHeight="1">
+    <row r="11" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="21" t="s">
         <v>35</v>
       </c>
@@ -911,7 +921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="22.5" customHeight="1">
+    <row r="12" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="9" t="s">
         <v>29</v>
       </c>
@@ -919,15 +929,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="22.5" customHeight="1">
+    <row r="13" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="20">
         <v>45180</v>
       </c>
       <c r="E13" s="19">
         <v>17500</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="22.5" customHeight="1">
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="9">
         <v>45256</v>
       </c>
@@ -936,7 +947,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="22.5" customHeight="1">
+    <row r="15" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="20">
         <v>45272</v>
       </c>
@@ -944,7 +955,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="22.5" customHeight="1">
+    <row r="16" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="9">
         <v>45274</v>
       </c>
@@ -952,7 +963,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="4:5" ht="22.5" customHeight="1">
+    <row r="17" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="20">
         <v>45275</v>
       </c>
@@ -960,43 +971,62 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="18" spans="4:5" ht="22.5" customHeight="1">
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-    </row>
-    <row r="19" spans="4:5" ht="22.5" customHeight="1"/>
-    <row r="20" spans="4:5" ht="22.5" customHeight="1">
-      <c r="D20" s="9" t="s">
+    <row r="18" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="20">
+        <v>45278</v>
+      </c>
+      <c r="E18" s="19">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+    </row>
+    <row r="21" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="4:5" ht="22.5" customHeight="1">
-      <c r="D21" s="20">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="20">
         <v>45180</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E23" s="19">
         <v>17380</v>
       </c>
     </row>
-    <row r="22" spans="4:5" ht="22.5" customHeight="1">
-      <c r="D22" s="9"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="4:5" ht="22.5" customHeight="1">
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="4:5" ht="22.5" customHeight="1">
+    <row r="24" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="9"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="4:5" ht="22.5" customHeight="1">
+    <row r="25" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="4:5" ht="15">
-      <c r="D26" s="10"/>
+    <row r="26" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="9"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="4:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="20"/>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="4:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1011,14 +1041,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E44"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="12"/>
     <col min="2" max="2" width="13.28515625" style="12" customWidth="1"/>
@@ -1028,10 +1058,10 @@
     <col min="6" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15">
+    <row r="1" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1">
+    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1069,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="2:5" ht="22.5" customHeight="1">
+    <row r="3" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>39</v>
       </c>
@@ -1049,7 +1079,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="22.5" customHeight="1">
+    <row r="4" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1087,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="2:5" ht="22.5" customHeight="1">
+    <row r="5" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
       <c r="C5" s="17" t="s">
         <v>2</v>
@@ -1065,7 +1095,7 @@
       <c r="D5" s="14"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="2:5" ht="22.5" customHeight="1">
+    <row r="6" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
@@ -1073,7 +1103,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="2:5" ht="22.5" customHeight="1">
+    <row r="7" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="14"/>
       <c r="D7" s="16" t="s">
@@ -1081,7 +1111,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5" ht="22.5" customHeight="1">
+    <row r="8" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="14"/>
       <c r="D8" s="16" t="s">
@@ -1089,7 +1119,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" ht="22.5" customHeight="1">
+    <row r="9" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="14"/>
       <c r="D9" s="17" t="s">
@@ -1097,7 +1127,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5" ht="22.5" customHeight="1">
+    <row r="10" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
       <c r="C10" s="17" t="s">
         <v>3</v>
@@ -1105,7 +1135,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" ht="22.5" customHeight="1">
+    <row r="11" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
       <c r="D11" s="16" t="s">
@@ -1113,7 +1143,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="22.5" customHeight="1">
+    <row r="12" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="16" t="s">
@@ -1121,7 +1151,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:5" ht="22.5" customHeight="1">
+    <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16" t="s">
@@ -1129,7 +1159,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:5" ht="22.5" customHeight="1">
+    <row r="14" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="16" t="s">
@@ -1137,7 +1167,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:5" ht="22.5" customHeight="1">
+    <row r="15" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
       <c r="D15" s="17" t="s">
@@ -1145,13 +1175,13 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="2:5" ht="22.5" customHeight="1">
+    <row r="16" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13"/>
       <c r="C16" s="16"/>
       <c r="D16" s="14"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" ht="22.5" customHeight="1">
+    <row r="17" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13"/>
       <c r="C17" s="17" t="s">
         <v>4</v>
@@ -1159,7 +1189,7 @@
       <c r="D17" s="14"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" ht="22.5" customHeight="1">
+    <row r="18" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16" t="s">
@@ -1167,7 +1197,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" ht="22.5" customHeight="1">
+    <row r="19" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16" t="s">
@@ -1175,7 +1205,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" ht="22.5" customHeight="1">
+    <row r="20" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
@@ -1183,7 +1213,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" ht="22.5" customHeight="1">
+    <row r="21" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
@@ -1191,7 +1221,7 @@
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="2:5" ht="22.5" customHeight="1">
+    <row r="22" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17" t="s">
@@ -1199,13 +1229,13 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:5" ht="22.5" customHeight="1">
+    <row r="23" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="13"/>
       <c r="C23" s="16"/>
       <c r="D23" s="14"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:5" ht="22.5" customHeight="1">
+    <row r="24" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
         <v>5</v>
       </c>
@@ -1213,7 +1243,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="2:5" ht="22.5" customHeight="1">
+    <row r="25" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
       <c r="C25" s="17" t="s">
         <v>6</v>
@@ -1221,7 +1251,7 @@
       <c r="D25" s="14"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="2:5" ht="22.5" customHeight="1">
+    <row r="26" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
@@ -1229,7 +1259,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="2:5" ht="22.5" customHeight="1">
+    <row r="27" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
@@ -1237,7 +1267,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="2:5" ht="22.5" customHeight="1">
+    <row r="28" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16" t="s">
@@ -1245,7 +1275,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="2:5" ht="22.5" customHeight="1">
+    <row r="29" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16" t="s">
@@ -1253,7 +1283,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="2:5" ht="22.5" customHeight="1">
+    <row r="30" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17" t="s">
@@ -1261,13 +1291,13 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="2:5" ht="22.5" customHeight="1">
+    <row r="31" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13"/>
       <c r="C31" s="16"/>
       <c r="D31" s="14"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="2:5" ht="22.5" customHeight="1">
+    <row r="32" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13"/>
       <c r="C32" s="17" t="s">
         <v>7</v>
@@ -1275,7 +1305,7 @@
       <c r="D32" s="14"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="2:5" ht="22.5" customHeight="1">
+    <row r="33" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16" t="s">
@@ -1283,7 +1313,7 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="2:5" ht="22.5" customHeight="1">
+    <row r="34" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="13"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16" t="s">
@@ -1291,7 +1321,7 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="2:5" ht="22.5" customHeight="1">
+    <row r="35" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="13"/>
       <c r="C35" s="16"/>
       <c r="D35" s="17" t="s">
@@ -1299,7 +1329,7 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="2:5" ht="22.5" customHeight="1">
+    <row r="36" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13"/>
       <c r="C36" s="16"/>
       <c r="D36" s="15" t="s">
@@ -1307,13 +1337,13 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="2:5" ht="22.5" customHeight="1">
+    <row r="37" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="13"/>
       <c r="C37" s="16"/>
       <c r="D37" s="14"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="2:5" ht="22.5" customHeight="1">
+    <row r="38" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="15" t="s">
         <v>8</v>
       </c>
@@ -1321,7 +1351,7 @@
       <c r="D38" s="14"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="2:5" ht="22.5" customHeight="1">
+    <row r="39" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="13"/>
       <c r="C39" s="16" t="s">
         <v>9</v>
@@ -1329,7 +1359,7 @@
       <c r="D39" s="14"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="2:5" ht="22.5" customHeight="1">
+    <row r="40" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="13"/>
       <c r="C40" s="16" t="s">
         <v>27</v>
@@ -1337,7 +1367,7 @@
       <c r="D40" s="14"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="2:5" ht="22.5" customHeight="1">
+    <row r="41" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="13"/>
       <c r="C41" s="16" t="s">
         <v>28</v>
@@ -1345,7 +1375,7 @@
       <c r="D41" s="14"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="2:5" ht="22.5" customHeight="1">
+    <row r="42" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13"/>
       <c r="C42" s="16" t="s">
         <v>40</v>
@@ -1353,13 +1383,13 @@
       <c r="D42" s="14"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="2:5" ht="22.5" customHeight="1">
+    <row r="43" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="13"/>
       <c r="C43" s="16"/>
       <c r="D43" s="14"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="2:5" ht="22.5" customHeight="1">
+    <row r="44" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="13"/>
       <c r="C44" s="17" t="s">
         <v>47</v>
@@ -1373,14 +1403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="3" width="12.7109375" style="4" customWidth="1"/>
@@ -1388,115 +1418,121 @@
     <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1"/>
-    <row r="3" spans="2:5">
+    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B5" s="35">
+    <row r="5" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="29">
         <v>45274</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="28">
         <v>480</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-    </row>
-    <row r="12" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-    </row>
-    <row r="13" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-    </row>
-    <row r="15" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-    </row>
-    <row r="16" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-    </row>
-    <row r="17" ht="22.5" customHeight="1"/>
-    <row r="18" ht="22.5" customHeight="1"/>
-    <row r="19" ht="22.5" customHeight="1"/>
-    <row r="20" ht="22.5" customHeight="1"/>
-    <row r="21" ht="22.5" customHeight="1"/>
-    <row r="22" ht="22.5" customHeight="1"/>
-    <row r="23" ht="22.5" customHeight="1"/>
-    <row r="24" ht="22.5" customHeight="1"/>
-    <row r="25" ht="22.5" customHeight="1"/>
+    <row r="6" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="29">
+        <v>45283</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>